<commit_message>
added missing CASE- values in data_coding_TPACK
</commit_message>
<xml_diff>
--- a/data/TPACK_Kodierung_ab1307.xlsx
+++ b/data/TPACK_Kodierung_ab1307.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25525"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="1695" documentId="11_92483E2D04E89AD36523F29B863E8C1851038389" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{13B97008-73C5-497F-B3EE-4B24AB3C91BA}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unitc-my.sharepoint.com/personal/m12aq01_cloud_uni-tuebingen_de/Documents/02-Projekte/03-M-TPACK/data_analysis/mTPACK/data/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="1698" documentId="11_92483E2D04E89AD36523F29B863E8C1851038389" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FE7360F1-AA29-4197-A12F-42ECA64C829D}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -2155,7 +2160,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2234,9 +2239,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -2255,7 +2258,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2553,13 +2556,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BK164"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A118" workbookViewId="0">
-      <selection activeCell="AO134" sqref="AO134"/>
+    <sheetView tabSelected="1" topLeftCell="A138" workbookViewId="0">
+      <selection activeCell="K147" sqref="K147"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:63" ht="15" customHeight="1">
+    <row r="1" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2714,7 +2717,7 @@
       <c r="BJ1" s="3"/>
       <c r="BK1" s="3"/>
     </row>
-    <row r="2" spans="1:63" ht="15" customHeight="1">
+    <row r="2" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>45</v>
       </c>
@@ -2805,7 +2808,7 @@
       <c r="BJ2" s="3"/>
       <c r="BK2" s="3"/>
     </row>
-    <row r="3" spans="1:63" ht="15" customHeight="1">
+    <row r="3" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>157</v>
       </c>
@@ -2926,7 +2929,7 @@
       <c r="BJ3" s="3"/>
       <c r="BK3" s="3"/>
     </row>
-    <row r="4" spans="1:63" ht="15" customHeight="1">
+    <row r="4" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>158</v>
       </c>
@@ -3047,7 +3050,7 @@
       <c r="BJ4" s="3"/>
       <c r="BK4" s="3"/>
     </row>
-    <row r="5" spans="1:63" ht="15" customHeight="1">
+    <row r="5" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>159</v>
       </c>
@@ -3076,7 +3079,7 @@
         <v>0</v>
       </c>
       <c r="J5" s="4">
-        <f t="shared" ref="J5:J68" si="1">SUM(G5:I5)</f>
+        <f t="shared" ref="J5:J64" si="1">SUM(G5:I5)</f>
         <v>0.5</v>
       </c>
       <c r="K5" s="1"/>
@@ -3097,7 +3100,7 @@
         <v>0</v>
       </c>
       <c r="T5" s="4">
-        <f t="shared" ref="T4:T67" si="2">SUM(Q5:S5)</f>
+        <f t="shared" ref="T5:T64" si="2">SUM(Q5:S5)</f>
         <v>0.5</v>
       </c>
       <c r="U5" s="3" t="s">
@@ -3171,7 +3174,7 @@
       <c r="BJ5" s="3"/>
       <c r="BK5" s="3"/>
     </row>
-    <row r="6" spans="1:63" ht="15" customHeight="1">
+    <row r="6" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>160</v>
       </c>
@@ -3249,7 +3252,7 @@
       <c r="BJ6" s="3"/>
       <c r="BK6" s="3"/>
     </row>
-    <row r="7" spans="1:63" ht="15" customHeight="1">
+    <row r="7" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>161</v>
       </c>
@@ -3315,7 +3318,7 @@
         <v>0</v>
       </c>
       <c r="Y7" s="4">
-        <f t="shared" ref="Y6:Y69" si="3">SUM(V7:X7)</f>
+        <f t="shared" ref="Y7:Y67" si="3">SUM(V7:X7)</f>
         <v>2</v>
       </c>
       <c r="Z7" s="3" t="s">
@@ -3373,7 +3376,7 @@
       <c r="BJ7" s="3"/>
       <c r="BK7" s="3"/>
     </row>
-    <row r="8" spans="1:63" ht="15" customHeight="1">
+    <row r="8" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>162</v>
       </c>
@@ -3448,7 +3451,7 @@
       <c r="BJ8" s="3"/>
       <c r="BK8" s="3"/>
     </row>
-    <row r="9" spans="1:63" ht="15" customHeight="1">
+    <row r="9" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>163</v>
       </c>
@@ -3569,7 +3572,7 @@
       <c r="BJ9" s="3"/>
       <c r="BK9" s="3"/>
     </row>
-    <row r="10" spans="1:63" ht="15" customHeight="1">
+    <row r="10" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>164</v>
       </c>
@@ -3693,7 +3696,7 @@
       <c r="BJ10" s="3"/>
       <c r="BK10" s="3"/>
     </row>
-    <row r="11" spans="1:63" ht="15" customHeight="1">
+    <row r="11" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>166</v>
       </c>
@@ -3817,7 +3820,7 @@
       <c r="BJ11" s="3"/>
       <c r="BK11" s="3"/>
     </row>
-    <row r="12" spans="1:63" ht="15" customHeight="1">
+    <row r="12" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>167</v>
       </c>
@@ -3892,7 +3895,7 @@
       <c r="BJ12" s="3"/>
       <c r="BK12" s="3"/>
     </row>
-    <row r="13" spans="1:63" ht="15" customHeight="1">
+    <row r="13" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>168</v>
       </c>
@@ -4013,7 +4016,7 @@
       <c r="BJ13" s="3"/>
       <c r="BK13" s="3"/>
     </row>
-    <row r="14" spans="1:63" ht="15" customHeight="1">
+    <row r="14" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>169</v>
       </c>
@@ -4140,7 +4143,7 @@
       <c r="BJ14" s="3"/>
       <c r="BK14" s="3"/>
     </row>
-    <row r="15" spans="1:63" ht="15" customHeight="1">
+    <row r="15" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>170</v>
       </c>
@@ -4258,7 +4261,7 @@
       <c r="BJ15" s="3"/>
       <c r="BK15" s="3"/>
     </row>
-    <row r="16" spans="1:63" ht="15" customHeight="1">
+    <row r="16" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <v>172</v>
       </c>
@@ -4385,7 +4388,7 @@
       <c r="BJ16" s="3"/>
       <c r="BK16" s="3"/>
     </row>
-    <row r="17" spans="1:63" ht="15" customHeight="1">
+    <row r="17" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
         <v>174</v>
       </c>
@@ -4506,7 +4509,7 @@
       <c r="BJ17" s="3"/>
       <c r="BK17" s="3"/>
     </row>
-    <row r="18" spans="1:63" ht="15" customHeight="1">
+    <row r="18" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
         <v>180</v>
       </c>
@@ -4630,7 +4633,7 @@
       <c r="BJ18" s="3"/>
       <c r="BK18" s="3"/>
     </row>
-    <row r="19" spans="1:63" ht="15" customHeight="1">
+    <row r="19" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
         <v>184</v>
       </c>
@@ -4732,7 +4735,7 @@
       <c r="BJ19" s="3"/>
       <c r="BK19" s="3"/>
     </row>
-    <row r="20" spans="1:63" ht="15" customHeight="1">
+    <row r="20" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
         <v>187</v>
       </c>
@@ -4815,7 +4818,7 @@
       <c r="BJ20" s="3"/>
       <c r="BK20" s="3"/>
     </row>
-    <row r="21" spans="1:63" ht="15" customHeight="1">
+    <row r="21" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
         <v>188</v>
       </c>
@@ -4933,7 +4936,7 @@
       <c r="BJ21" s="3"/>
       <c r="BK21" s="3"/>
     </row>
-    <row r="22" spans="1:63" ht="15" customHeight="1">
+    <row r="22" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="1">
         <v>190</v>
       </c>
@@ -5057,7 +5060,7 @@
       <c r="BJ22" s="3"/>
       <c r="BK22" s="3"/>
     </row>
-    <row r="23" spans="1:63" ht="15" customHeight="1">
+    <row r="23" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="1">
         <v>191</v>
       </c>
@@ -5184,7 +5187,7 @@
       <c r="BJ23" s="3"/>
       <c r="BK23" s="3"/>
     </row>
-    <row r="24" spans="1:63" ht="15" customHeight="1">
+    <row r="24" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="1">
         <v>194</v>
       </c>
@@ -5308,7 +5311,7 @@
       <c r="BJ24" s="3"/>
       <c r="BK24" s="3"/>
     </row>
-    <row r="25" spans="1:63" ht="15" customHeight="1">
+    <row r="25" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="1">
         <v>195</v>
       </c>
@@ -5426,7 +5429,7 @@
       <c r="BJ25" s="3"/>
       <c r="BK25" s="3"/>
     </row>
-    <row r="26" spans="1:63" ht="15" customHeight="1">
+    <row r="26" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="1">
         <v>199</v>
       </c>
@@ -5550,7 +5553,7 @@
       <c r="BJ26" s="3"/>
       <c r="BK26" s="3"/>
     </row>
-    <row r="27" spans="1:63" ht="15" customHeight="1">
+    <row r="27" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="1">
         <v>201</v>
       </c>
@@ -5674,7 +5677,7 @@
       <c r="BJ27" s="3"/>
       <c r="BK27" s="3"/>
     </row>
-    <row r="28" spans="1:63" ht="15" customHeight="1">
+    <row r="28" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="1">
         <v>202</v>
       </c>
@@ -5795,7 +5798,7 @@
       <c r="BJ28" s="3"/>
       <c r="BK28" s="3"/>
     </row>
-    <row r="29" spans="1:63" ht="15" customHeight="1">
+    <row r="29" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="1">
         <v>204</v>
       </c>
@@ -5897,7 +5900,7 @@
       <c r="BJ29" s="3"/>
       <c r="BK29" s="3"/>
     </row>
-    <row r="30" spans="1:63" ht="15" customHeight="1">
+    <row r="30" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="1">
         <v>205</v>
       </c>
@@ -6018,7 +6021,7 @@
       <c r="BJ30" s="3"/>
       <c r="BK30" s="3"/>
     </row>
-    <row r="31" spans="1:63" ht="15" customHeight="1">
+    <row r="31" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="1">
         <v>206</v>
       </c>
@@ -6142,7 +6145,7 @@
       <c r="BJ31" s="3"/>
       <c r="BK31" s="3"/>
     </row>
-    <row r="32" spans="1:63" ht="15" customHeight="1">
+    <row r="32" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="1">
         <v>209</v>
       </c>
@@ -6263,7 +6266,7 @@
       <c r="BJ32" s="3"/>
       <c r="BK32" s="3"/>
     </row>
-    <row r="33" spans="1:63" ht="15" customHeight="1">
+    <row r="33" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="1">
         <v>211</v>
       </c>
@@ -6384,7 +6387,7 @@
       <c r="BJ33" s="3"/>
       <c r="BK33" s="3"/>
     </row>
-    <row r="34" spans="1:63" ht="15" customHeight="1">
+    <row r="34" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="1">
         <v>216</v>
       </c>
@@ -6508,7 +6511,7 @@
       <c r="BJ34" s="3"/>
       <c r="BK34" s="3"/>
     </row>
-    <row r="35" spans="1:63" ht="15" customHeight="1">
+    <row r="35" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="1">
         <v>218</v>
       </c>
@@ -6632,7 +6635,7 @@
       <c r="BJ35" s="3"/>
       <c r="BK35" s="3"/>
     </row>
-    <row r="36" spans="1:63" ht="15" customHeight="1">
+    <row r="36" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="1">
         <v>219</v>
       </c>
@@ -6707,7 +6710,7 @@
       <c r="BJ36" s="3"/>
       <c r="BK36" s="3"/>
     </row>
-    <row r="37" spans="1:63" ht="15" customHeight="1">
+    <row r="37" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="1">
         <v>220</v>
       </c>
@@ -6823,7 +6826,7 @@
       <c r="BJ37" s="3"/>
       <c r="BK37" s="3"/>
     </row>
-    <row r="38" spans="1:63" ht="15" customHeight="1">
+    <row r="38" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="1">
         <v>224</v>
       </c>
@@ -6912,7 +6915,7 @@
       <c r="BJ38" s="3"/>
       <c r="BK38" s="3"/>
     </row>
-    <row r="39" spans="1:63" ht="15" customHeight="1">
+    <row r="39" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="1">
         <v>227</v>
       </c>
@@ -7025,8 +7028,8 @@
       <c r="BJ39" s="3"/>
       <c r="BK39" s="3"/>
     </row>
-    <row r="40" spans="1:63" ht="15" customHeight="1">
-      <c r="A40" s="1">
+    <row r="40" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="10">
         <v>231</v>
       </c>
       <c r="B40" s="2"/>
@@ -7135,8 +7138,10 @@
       <c r="BJ40" s="3"/>
       <c r="BK40" s="3"/>
     </row>
-    <row r="41" spans="1:63" ht="15" customHeight="1">
-      <c r="A41" s="3"/>
+    <row r="41" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="10">
+        <v>235</v>
+      </c>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
@@ -7200,8 +7205,10 @@
       <c r="BJ41" s="3"/>
       <c r="BK41" s="3"/>
     </row>
-    <row r="42" spans="1:63" ht="15" customHeight="1">
-      <c r="A42" s="3"/>
+    <row r="42" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A42" s="10">
+        <v>236</v>
+      </c>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
@@ -7314,8 +7321,10 @@
       <c r="BJ42" s="3"/>
       <c r="BK42" s="3"/>
     </row>
-    <row r="43" spans="1:63" ht="15" customHeight="1">
-      <c r="A43" s="3"/>
+    <row r="43" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="10">
+        <v>237</v>
+      </c>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>
@@ -7382,8 +7391,10 @@
       <c r="BJ43" s="3"/>
       <c r="BK43" s="3"/>
     </row>
-    <row r="44" spans="1:63" ht="15" customHeight="1">
-      <c r="A44" s="3"/>
+    <row r="44" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A44" s="10">
+        <v>241</v>
+      </c>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
       <c r="D44" s="2"/>
@@ -7499,8 +7510,10 @@
       <c r="BJ44" s="3"/>
       <c r="BK44" s="3"/>
     </row>
-    <row r="45" spans="1:63" ht="15" customHeight="1">
-      <c r="A45" s="3"/>
+    <row r="45" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="10">
+        <v>245</v>
+      </c>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
       <c r="D45" s="2"/>
@@ -7564,8 +7577,10 @@
       <c r="BJ45" s="3"/>
       <c r="BK45" s="3"/>
     </row>
-    <row r="46" spans="1:63" ht="15" customHeight="1">
-      <c r="A46" s="3"/>
+    <row r="46" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A46" s="10">
+        <v>246</v>
+      </c>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
       <c r="D46" s="2"/>
@@ -7675,8 +7690,10 @@
       <c r="BJ46" s="3"/>
       <c r="BK46" s="3"/>
     </row>
-    <row r="47" spans="1:63" ht="15" customHeight="1">
-      <c r="A47" s="3"/>
+    <row r="47" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A47" s="10">
+        <v>249</v>
+      </c>
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
       <c r="D47" s="2"/>
@@ -7740,8 +7757,10 @@
       <c r="BJ47" s="3"/>
       <c r="BK47" s="3"/>
     </row>
-    <row r="48" spans="1:63" ht="15" customHeight="1">
-      <c r="A48" s="3"/>
+    <row r="48" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A48" s="10">
+        <v>250</v>
+      </c>
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
       <c r="D48" s="2"/>
@@ -7851,8 +7870,10 @@
       <c r="BJ48" s="3"/>
       <c r="BK48" s="3"/>
     </row>
-    <row r="49" spans="1:63" ht="15" customHeight="1">
-      <c r="A49" s="3"/>
+    <row r="49" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A49" s="10">
+        <v>251</v>
+      </c>
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
       <c r="D49" s="2"/>
@@ -7916,8 +7937,10 @@
       <c r="BJ49" s="3"/>
       <c r="BK49" s="3"/>
     </row>
-    <row r="50" spans="1:63" ht="15" customHeight="1">
-      <c r="A50" s="3"/>
+    <row r="50" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A50" s="10">
+        <v>253</v>
+      </c>
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
       <c r="D50" s="2"/>
@@ -8030,8 +8053,10 @@
       <c r="BJ50" s="3"/>
       <c r="BK50" s="3"/>
     </row>
-    <row r="51" spans="1:63" ht="15" customHeight="1">
-      <c r="A51" s="3"/>
+    <row r="51" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A51" s="10">
+        <v>255</v>
+      </c>
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>
       <c r="D51" s="2"/>
@@ -8095,8 +8120,10 @@
       <c r="BJ51" s="3"/>
       <c r="BK51" s="3"/>
     </row>
-    <row r="52" spans="1:63" ht="15" customHeight="1">
-      <c r="A52" s="3"/>
+    <row r="52" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A52" s="10">
+        <v>257</v>
+      </c>
       <c r="B52" s="2"/>
       <c r="C52" s="2"/>
       <c r="D52" s="2"/>
@@ -8206,8 +8233,10 @@
       <c r="BJ52" s="3"/>
       <c r="BK52" s="3"/>
     </row>
-    <row r="53" spans="1:63" ht="15" customHeight="1">
-      <c r="A53" s="3"/>
+    <row r="53" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A53" s="10">
+        <v>259</v>
+      </c>
       <c r="B53" s="2"/>
       <c r="C53" s="2"/>
       <c r="D53" s="2"/>
@@ -8315,8 +8344,10 @@
       <c r="BJ53" s="3"/>
       <c r="BK53" s="3"/>
     </row>
-    <row r="54" spans="1:63" ht="15" customHeight="1">
-      <c r="A54" s="3"/>
+    <row r="54" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A54" s="10">
+        <v>262</v>
+      </c>
       <c r="B54" s="2"/>
       <c r="C54" s="2"/>
       <c r="D54" s="2"/>
@@ -8380,8 +8411,10 @@
       <c r="BJ54" s="3"/>
       <c r="BK54" s="3"/>
     </row>
-    <row r="55" spans="1:63" ht="15" customHeight="1">
-      <c r="A55" s="3"/>
+    <row r="55" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A55" s="10">
+        <v>267</v>
+      </c>
       <c r="B55" s="2"/>
       <c r="C55" s="2"/>
       <c r="D55" s="2"/>
@@ -8497,8 +8530,10 @@
       <c r="BJ55" s="3"/>
       <c r="BK55" s="3"/>
     </row>
-    <row r="56" spans="1:63" ht="15" customHeight="1">
-      <c r="A56" s="3"/>
+    <row r="56" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A56" s="10">
+        <v>269</v>
+      </c>
       <c r="B56" s="2"/>
       <c r="C56" s="2"/>
       <c r="D56" s="2"/>
@@ -8605,8 +8640,10 @@
       <c r="BJ56" s="3"/>
       <c r="BK56" s="3"/>
     </row>
-    <row r="57" spans="1:63" ht="15" customHeight="1">
-      <c r="A57" s="3"/>
+    <row r="57" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A57" s="10">
+        <v>270</v>
+      </c>
       <c r="B57" s="2"/>
       <c r="C57" s="2"/>
       <c r="D57" s="2"/>
@@ -8670,8 +8707,10 @@
       <c r="BJ57" s="3"/>
       <c r="BK57" s="3"/>
     </row>
-    <row r="58" spans="1:63" ht="15" customHeight="1">
-      <c r="A58" s="3"/>
+    <row r="58" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A58" s="10">
+        <v>271</v>
+      </c>
       <c r="B58" s="2"/>
       <c r="C58" s="2"/>
       <c r="D58" s="2"/>
@@ -8784,8 +8823,10 @@
       <c r="BJ58" s="3"/>
       <c r="BK58" s="3"/>
     </row>
-    <row r="59" spans="1:63" ht="15" customHeight="1">
-      <c r="A59" s="3"/>
+    <row r="59" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A59" s="10">
+        <v>275</v>
+      </c>
       <c r="B59" s="2"/>
       <c r="C59" s="2"/>
       <c r="D59" s="2"/>
@@ -8898,8 +8939,10 @@
       <c r="BJ59" s="3"/>
       <c r="BK59" s="3"/>
     </row>
-    <row r="60" spans="1:63" ht="15" customHeight="1">
-      <c r="A60" s="3"/>
+    <row r="60" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A60" s="10">
+        <v>278</v>
+      </c>
       <c r="B60" s="2"/>
       <c r="C60" s="2"/>
       <c r="D60" s="2"/>
@@ -9012,8 +9055,10 @@
       <c r="BJ60" s="3"/>
       <c r="BK60" s="3"/>
     </row>
-    <row r="61" spans="1:63" ht="15" customHeight="1">
-      <c r="A61" s="3"/>
+    <row r="61" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A61" s="10">
+        <v>280</v>
+      </c>
       <c r="B61" s="2"/>
       <c r="C61" s="2"/>
       <c r="D61" s="2"/>
@@ -9123,8 +9168,10 @@
       <c r="BJ61" s="3"/>
       <c r="BK61" s="3"/>
     </row>
-    <row r="62" spans="1:63" ht="15" customHeight="1">
-      <c r="A62" s="3"/>
+    <row r="62" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A62" s="10">
+        <v>284</v>
+      </c>
       <c r="B62" s="2"/>
       <c r="C62" s="2"/>
       <c r="D62" s="2"/>
@@ -9237,8 +9284,10 @@
       <c r="BJ62" s="3"/>
       <c r="BK62" s="3"/>
     </row>
-    <row r="63" spans="1:63" ht="15" customHeight="1">
-      <c r="A63" s="3"/>
+    <row r="63" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A63" s="10">
+        <v>285</v>
+      </c>
       <c r="B63" s="2"/>
       <c r="C63" s="2"/>
       <c r="D63" s="2"/>
@@ -9302,8 +9351,10 @@
       <c r="BJ63" s="3"/>
       <c r="BK63" s="3"/>
     </row>
-    <row r="64" spans="1:63" ht="15" customHeight="1">
-      <c r="A64" s="3"/>
+    <row r="64" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A64" s="10">
+        <v>287</v>
+      </c>
       <c r="B64" s="2"/>
       <c r="C64" s="2"/>
       <c r="D64" s="2"/>
@@ -9416,8 +9467,10 @@
       <c r="BJ64" s="3"/>
       <c r="BK64" s="3"/>
     </row>
-    <row r="65" spans="1:63" ht="15" customHeight="1">
-      <c r="A65" s="3"/>
+    <row r="65" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A65" s="10">
+        <v>289</v>
+      </c>
       <c r="B65" s="2"/>
       <c r="C65" s="2"/>
       <c r="D65" s="2"/>
@@ -9481,8 +9534,10 @@
       <c r="BJ65" s="3"/>
       <c r="BK65" s="3"/>
     </row>
-    <row r="66" spans="1:63" ht="15" customHeight="1">
-      <c r="A66" s="3"/>
+    <row r="66" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A66" s="10">
+        <v>290</v>
+      </c>
       <c r="B66" s="2"/>
       <c r="C66" s="2"/>
       <c r="D66" s="2"/>
@@ -9573,8 +9628,10 @@
       <c r="BJ66" s="3"/>
       <c r="BK66" s="3"/>
     </row>
-    <row r="67" spans="1:63" ht="15" customHeight="1">
-      <c r="A67" s="3"/>
+    <row r="67" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A67" s="10">
+        <v>292</v>
+      </c>
       <c r="B67" s="2"/>
       <c r="C67" s="2"/>
       <c r="D67" s="2"/>
@@ -9684,8 +9741,10 @@
       <c r="BJ67" s="3"/>
       <c r="BK67" s="3"/>
     </row>
-    <row r="68" spans="1:63" ht="15" customHeight="1">
-      <c r="A68" s="3"/>
+    <row r="68" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A68" s="10">
+        <v>293</v>
+      </c>
       <c r="B68" s="2"/>
       <c r="C68" s="2"/>
       <c r="D68" s="2"/>
@@ -9749,8 +9808,10 @@
       <c r="BJ68" s="3"/>
       <c r="BK68" s="3"/>
     </row>
-    <row r="69" spans="1:63" ht="15" customHeight="1">
-      <c r="A69" s="3"/>
+    <row r="69" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A69" s="10">
+        <v>294</v>
+      </c>
       <c r="B69" s="2"/>
       <c r="C69" s="2"/>
       <c r="D69" s="2"/>
@@ -9778,7 +9839,7 @@
         <v>0</v>
       </c>
       <c r="T69" s="4">
-        <f t="shared" ref="T68:T131" si="4">SUM(Q69:S69)</f>
+        <f t="shared" ref="T69:T129" si="4">SUM(Q69:S69)</f>
         <v>1.5</v>
       </c>
       <c r="U69" s="3"/>
@@ -9857,8 +9918,10 @@
       <c r="BJ69" s="3"/>
       <c r="BK69" s="3"/>
     </row>
-    <row r="70" spans="1:63" ht="15" customHeight="1">
-      <c r="A70" s="3"/>
+    <row r="70" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A70" s="10">
+        <v>299</v>
+      </c>
       <c r="B70" s="2"/>
       <c r="C70" s="2"/>
       <c r="D70" s="2"/>
@@ -9876,7 +9939,7 @@
         <v>0</v>
       </c>
       <c r="J70" s="4">
-        <f t="shared" ref="J69:J132" si="5">SUM(G70:I70)</f>
+        <f t="shared" ref="J70:J132" si="5">SUM(G70:I70)</f>
         <v>1</v>
       </c>
       <c r="K70" s="3" t="s">
@@ -9892,7 +9955,7 @@
         <v>0</v>
       </c>
       <c r="O70" s="4">
-        <f t="shared" ref="O68:O131" si="6">SUM(L70:N70)</f>
+        <f t="shared" ref="O70:O131" si="6">SUM(L70:N70)</f>
         <v>1.5</v>
       </c>
       <c r="P70" s="3"/>
@@ -9971,8 +10034,10 @@
       <c r="BJ70" s="3"/>
       <c r="BK70" s="3"/>
     </row>
-    <row r="71" spans="1:63" ht="15" customHeight="1">
-      <c r="A71" s="3"/>
+    <row r="71" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A71" s="10">
+        <v>301</v>
+      </c>
       <c r="B71" s="2"/>
       <c r="C71" s="2"/>
       <c r="D71" s="2"/>
@@ -10085,8 +10150,10 @@
       <c r="BJ71" s="3"/>
       <c r="BK71" s="3"/>
     </row>
-    <row r="72" spans="1:63" ht="15" customHeight="1">
-      <c r="A72" s="3"/>
+    <row r="72" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A72" s="10">
+        <v>302</v>
+      </c>
       <c r="B72" s="2"/>
       <c r="C72" s="2"/>
       <c r="D72" s="2"/>
@@ -10196,8 +10263,10 @@
       <c r="BJ72" s="3"/>
       <c r="BK72" s="3"/>
     </row>
-    <row r="73" spans="1:63" ht="15" customHeight="1">
-      <c r="A73" s="3"/>
+    <row r="73" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A73" s="10">
+        <v>303</v>
+      </c>
       <c r="B73" s="2"/>
       <c r="C73" s="2"/>
       <c r="D73" s="2"/>
@@ -10310,8 +10379,10 @@
       <c r="BJ73" s="3"/>
       <c r="BK73" s="3"/>
     </row>
-    <row r="74" spans="1:63" ht="15" customHeight="1">
-      <c r="A74" s="3"/>
+    <row r="74" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A74" s="10">
+        <v>305</v>
+      </c>
       <c r="B74" s="2"/>
       <c r="C74" s="2"/>
       <c r="D74" s="2"/>
@@ -10421,8 +10492,10 @@
       <c r="BJ74" s="3"/>
       <c r="BK74" s="3"/>
     </row>
-    <row r="75" spans="1:63" ht="15" customHeight="1">
-      <c r="A75" s="3"/>
+    <row r="75" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A75" s="10">
+        <v>309</v>
+      </c>
       <c r="B75" s="2"/>
       <c r="C75" s="2"/>
       <c r="D75" s="2"/>
@@ -10538,8 +10611,10 @@
       <c r="BJ75" s="3"/>
       <c r="BK75" s="3"/>
     </row>
-    <row r="76" spans="1:63" ht="15" customHeight="1">
-      <c r="A76" s="3"/>
+    <row r="76" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A76" s="10">
+        <v>318</v>
+      </c>
       <c r="B76" s="2"/>
       <c r="C76" s="2"/>
       <c r="D76" s="2"/>
@@ -10649,8 +10724,10 @@
       <c r="BJ76" s="3"/>
       <c r="BK76" s="3"/>
     </row>
-    <row r="77" spans="1:63" ht="15" customHeight="1">
-      <c r="A77" s="3"/>
+    <row r="77" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A77" s="10">
+        <v>322</v>
+      </c>
       <c r="B77" s="2"/>
       <c r="C77" s="2"/>
       <c r="D77" s="2"/>
@@ -10714,8 +10791,10 @@
       <c r="BJ77" s="3"/>
       <c r="BK77" s="3"/>
     </row>
-    <row r="78" spans="1:63" ht="15" customHeight="1">
-      <c r="A78" s="3"/>
+    <row r="78" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A78" s="10">
+        <v>323</v>
+      </c>
       <c r="B78" s="2"/>
       <c r="C78" s="2"/>
       <c r="D78" s="2"/>
@@ -10825,8 +10904,10 @@
       <c r="BJ78" s="3"/>
       <c r="BK78" s="3"/>
     </row>
-    <row r="79" spans="1:63" ht="15" customHeight="1">
-      <c r="A79" s="3"/>
+    <row r="79" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A79" s="10">
+        <v>324</v>
+      </c>
       <c r="B79" s="2"/>
       <c r="C79" s="2"/>
       <c r="D79" s="2"/>
@@ -10939,8 +11020,10 @@
       <c r="BJ79" s="3"/>
       <c r="BK79" s="3"/>
     </row>
-    <row r="80" spans="1:63" ht="15" customHeight="1">
-      <c r="A80" s="3"/>
+    <row r="80" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A80" s="10">
+        <v>325</v>
+      </c>
       <c r="B80" s="2"/>
       <c r="C80" s="2"/>
       <c r="D80" s="2"/>
@@ -11050,8 +11133,10 @@
       <c r="BJ80" s="3"/>
       <c r="BK80" s="3"/>
     </row>
-    <row r="81" spans="1:63" ht="15" customHeight="1">
-      <c r="A81" s="3"/>
+    <row r="81" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A81" s="10">
+        <v>331</v>
+      </c>
       <c r="B81" s="2"/>
       <c r="C81" s="2"/>
       <c r="D81" s="2"/>
@@ -11164,8 +11249,10 @@
       <c r="BJ81" s="3"/>
       <c r="BK81" s="3"/>
     </row>
-    <row r="82" spans="1:63" ht="15" customHeight="1">
-      <c r="A82" s="3"/>
+    <row r="82" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A82" s="10">
+        <v>332</v>
+      </c>
       <c r="B82" s="2"/>
       <c r="C82" s="2"/>
       <c r="D82" s="2"/>
@@ -11275,8 +11362,10 @@
       <c r="BJ82" s="3"/>
       <c r="BK82" s="3"/>
     </row>
-    <row r="83" spans="1:63" ht="15" customHeight="1">
-      <c r="A83" s="3"/>
+    <row r="83" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A83" s="10">
+        <v>333</v>
+      </c>
       <c r="B83" s="2"/>
       <c r="C83" s="2"/>
       <c r="D83" s="2"/>
@@ -11386,8 +11475,10 @@
       <c r="BJ83" s="3"/>
       <c r="BK83" s="3"/>
     </row>
-    <row r="84" spans="1:63" ht="15" customHeight="1">
-      <c r="A84" s="3"/>
+    <row r="84" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A84" s="10">
+        <v>335</v>
+      </c>
       <c r="B84" s="2"/>
       <c r="C84" s="2"/>
       <c r="D84" s="2"/>
@@ -11497,8 +11588,10 @@
       <c r="BJ84" s="3"/>
       <c r="BK84" s="3"/>
     </row>
-    <row r="85" spans="1:63" ht="15" customHeight="1">
-      <c r="A85" s="3"/>
+    <row r="85" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A85" s="10">
+        <v>336</v>
+      </c>
       <c r="B85" s="2"/>
       <c r="C85" s="2"/>
       <c r="D85" s="2"/>
@@ -11614,8 +11707,10 @@
       <c r="BJ85" s="3"/>
       <c r="BK85" s="3"/>
     </row>
-    <row r="86" spans="1:63" ht="15" customHeight="1">
-      <c r="A86" s="3"/>
+    <row r="86" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A86" s="10">
+        <v>338</v>
+      </c>
       <c r="B86" s="2"/>
       <c r="C86" s="2"/>
       <c r="D86" s="2"/>
@@ -11728,8 +11823,10 @@
       <c r="BJ86" s="3"/>
       <c r="BK86" s="3"/>
     </row>
-    <row r="87" spans="1:63" ht="15" customHeight="1">
-      <c r="A87" s="3"/>
+    <row r="87" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A87" s="10">
+        <v>341</v>
+      </c>
       <c r="B87" s="2"/>
       <c r="C87" s="2"/>
       <c r="D87" s="2"/>
@@ -11839,8 +11936,10 @@
       <c r="BJ87" s="3"/>
       <c r="BK87" s="3"/>
     </row>
-    <row r="88" spans="1:63" ht="15" customHeight="1">
-      <c r="A88" s="3"/>
+    <row r="88" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A88" s="10">
+        <v>343</v>
+      </c>
       <c r="B88" s="2"/>
       <c r="C88" s="2"/>
       <c r="D88" s="2"/>
@@ -11947,8 +12046,10 @@
       <c r="BJ88" s="3"/>
       <c r="BK88" s="3"/>
     </row>
-    <row r="89" spans="1:63" ht="15" customHeight="1">
-      <c r="A89" s="3"/>
+    <row r="89" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A89" s="10">
+        <v>345</v>
+      </c>
       <c r="B89" s="2"/>
       <c r="C89" s="2"/>
       <c r="D89" s="2"/>
@@ -12064,8 +12165,10 @@
       <c r="BJ89" s="3"/>
       <c r="BK89" s="3"/>
     </row>
-    <row r="90" spans="1:63" ht="15" customHeight="1">
-      <c r="A90" s="3"/>
+    <row r="90" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A90" s="10">
+        <v>346</v>
+      </c>
       <c r="B90" s="2"/>
       <c r="C90" s="2"/>
       <c r="D90" s="2"/>
@@ -12178,8 +12281,10 @@
       <c r="BJ90" s="3"/>
       <c r="BK90" s="3"/>
     </row>
-    <row r="91" spans="1:63" ht="15" customHeight="1">
-      <c r="A91" s="3"/>
+    <row r="91" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A91" s="10">
+        <v>354</v>
+      </c>
       <c r="B91" s="2"/>
       <c r="C91" s="2"/>
       <c r="D91" s="2"/>
@@ -12289,8 +12394,10 @@
       <c r="BJ91" s="3"/>
       <c r="BK91" s="3"/>
     </row>
-    <row r="92" spans="1:63" ht="15" customHeight="1">
-      <c r="A92" s="3"/>
+    <row r="92" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A92" s="10">
+        <v>357</v>
+      </c>
       <c r="B92" s="2"/>
       <c r="C92" s="2"/>
       <c r="D92" s="2"/>
@@ -12362,8 +12469,10 @@
       <c r="BJ92" s="3"/>
       <c r="BK92" s="3"/>
     </row>
-    <row r="93" spans="1:63" ht="15" customHeight="1">
-      <c r="A93" s="3"/>
+    <row r="93" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A93" s="10">
+        <v>358</v>
+      </c>
       <c r="B93" s="2"/>
       <c r="C93" s="2"/>
       <c r="D93" s="2"/>
@@ -12476,8 +12585,10 @@
       <c r="BJ93" s="3"/>
       <c r="BK93" s="3"/>
     </row>
-    <row r="94" spans="1:63" ht="15" customHeight="1">
-      <c r="A94" s="3"/>
+    <row r="94" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A94" s="10">
+        <v>359</v>
+      </c>
       <c r="B94" s="2"/>
       <c r="C94" s="2"/>
       <c r="D94" s="2"/>
@@ -12590,8 +12701,10 @@
       <c r="BJ94" s="3"/>
       <c r="BK94" s="3"/>
     </row>
-    <row r="95" spans="1:63" ht="15" customHeight="1">
-      <c r="A95" s="3"/>
+    <row r="95" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A95" s="10">
+        <v>362</v>
+      </c>
       <c r="B95" s="2"/>
       <c r="C95" s="2"/>
       <c r="D95" s="2"/>
@@ -12701,8 +12814,10 @@
       <c r="BJ95" s="3"/>
       <c r="BK95" s="3"/>
     </row>
-    <row r="96" spans="1:63" ht="15" customHeight="1">
-      <c r="A96" s="3"/>
+    <row r="96" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A96" s="10">
+        <v>365</v>
+      </c>
       <c r="B96" s="2"/>
       <c r="C96" s="2"/>
       <c r="D96" s="2"/>
@@ -12815,8 +12930,10 @@
       <c r="BJ96" s="3"/>
       <c r="BK96" s="3"/>
     </row>
-    <row r="97" spans="1:63" ht="15" customHeight="1">
-      <c r="A97" s="3"/>
+    <row r="97" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A97" s="10">
+        <v>367</v>
+      </c>
       <c r="B97" s="2"/>
       <c r="C97" s="2"/>
       <c r="D97" s="2"/>
@@ -12923,8 +13040,10 @@
       <c r="BJ97" s="3"/>
       <c r="BK97" s="3"/>
     </row>
-    <row r="98" spans="1:63" ht="15" customHeight="1">
-      <c r="A98" s="3"/>
+    <row r="98" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A98" s="10">
+        <v>371</v>
+      </c>
       <c r="B98" s="2"/>
       <c r="C98" s="2"/>
       <c r="D98" s="2"/>
@@ -13037,8 +13156,10 @@
       <c r="BJ98" s="3"/>
       <c r="BK98" s="3"/>
     </row>
-    <row r="99" spans="1:63" ht="15" customHeight="1">
-      <c r="A99" s="3"/>
+    <row r="99" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A99" s="10">
+        <v>372</v>
+      </c>
       <c r="B99" s="2"/>
       <c r="C99" s="2"/>
       <c r="D99" s="2"/>
@@ -13148,8 +13269,10 @@
       <c r="BJ99" s="3"/>
       <c r="BK99" s="3"/>
     </row>
-    <row r="100" spans="1:63" ht="15" customHeight="1">
-      <c r="A100" s="3"/>
+    <row r="100" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A100" s="10">
+        <v>375</v>
+      </c>
       <c r="B100" s="2"/>
       <c r="C100" s="2"/>
       <c r="D100" s="2"/>
@@ -13262,8 +13385,10 @@
       <c r="BJ100" s="3"/>
       <c r="BK100" s="3"/>
     </row>
-    <row r="101" spans="1:63" ht="15" customHeight="1">
-      <c r="A101" s="3"/>
+    <row r="101" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A101" s="10">
+        <v>376</v>
+      </c>
       <c r="B101" s="2"/>
       <c r="C101" s="2"/>
       <c r="D101" s="2"/>
@@ -13373,8 +13498,10 @@
       <c r="BJ101" s="3"/>
       <c r="BK101" s="3"/>
     </row>
-    <row r="102" spans="1:63" ht="15" customHeight="1">
-      <c r="A102" s="3"/>
+    <row r="102" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A102" s="10">
+        <v>378</v>
+      </c>
       <c r="B102" s="2"/>
       <c r="C102" s="2"/>
       <c r="D102" s="2"/>
@@ -13438,8 +13565,10 @@
       <c r="BJ102" s="3"/>
       <c r="BK102" s="3"/>
     </row>
-    <row r="103" spans="1:63" ht="15" customHeight="1">
-      <c r="A103" s="3"/>
+    <row r="103" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A103" s="10">
+        <v>392</v>
+      </c>
       <c r="B103" s="2"/>
       <c r="C103" s="2"/>
       <c r="D103" s="2"/>
@@ -13549,8 +13678,10 @@
       <c r="BJ103" s="3"/>
       <c r="BK103" s="3"/>
     </row>
-    <row r="104" spans="1:63" ht="15" customHeight="1">
-      <c r="A104" s="3"/>
+    <row r="104" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A104" s="10">
+        <v>402</v>
+      </c>
       <c r="B104" s="2"/>
       <c r="C104" s="2"/>
       <c r="D104" s="2"/>
@@ -13666,8 +13797,10 @@
       <c r="BJ104" s="3"/>
       <c r="BK104" s="3"/>
     </row>
-    <row r="105" spans="1:63" ht="15" customHeight="1">
-      <c r="A105" s="3"/>
+    <row r="105" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A105" s="10">
+        <v>408</v>
+      </c>
       <c r="B105" s="2"/>
       <c r="C105" s="2"/>
       <c r="D105" s="2"/>
@@ -13731,8 +13864,10 @@
       <c r="BJ105" s="3"/>
       <c r="BK105" s="3"/>
     </row>
-    <row r="106" spans="1:63" ht="15" customHeight="1">
-      <c r="A106" s="3"/>
+    <row r="106" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A106" s="10">
+        <v>409</v>
+      </c>
       <c r="B106" s="2"/>
       <c r="C106" s="2"/>
       <c r="D106" s="2"/>
@@ -13842,8 +13977,10 @@
       <c r="BJ106" s="3"/>
       <c r="BK106" s="3"/>
     </row>
-    <row r="107" spans="1:63" ht="15" customHeight="1">
-      <c r="A107" s="3"/>
+    <row r="107" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A107" s="10">
+        <v>410</v>
+      </c>
       <c r="B107" s="2"/>
       <c r="C107" s="2"/>
       <c r="D107" s="2"/>
@@ -13950,8 +14087,10 @@
       <c r="BJ107" s="3"/>
       <c r="BK107" s="3"/>
     </row>
-    <row r="108" spans="1:63" ht="15" customHeight="1">
-      <c r="A108" s="3"/>
+    <row r="108" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A108" s="10">
+        <v>411</v>
+      </c>
       <c r="B108" s="2"/>
       <c r="C108" s="2"/>
       <c r="D108" s="2"/>
@@ -14061,8 +14200,10 @@
       <c r="BJ108" s="3"/>
       <c r="BK108" s="3"/>
     </row>
-    <row r="109" spans="1:63" ht="15" customHeight="1">
-      <c r="A109" s="3"/>
+    <row r="109" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A109" s="10">
+        <v>419</v>
+      </c>
       <c r="B109" s="2"/>
       <c r="C109" s="2"/>
       <c r="D109" s="2"/>
@@ -14126,8 +14267,10 @@
       <c r="BJ109" s="3"/>
       <c r="BK109" s="3"/>
     </row>
-    <row r="110" spans="1:63" ht="15" customHeight="1">
-      <c r="A110" s="3"/>
+    <row r="110" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A110" s="10">
+        <v>420</v>
+      </c>
       <c r="B110" s="2"/>
       <c r="C110" s="2"/>
       <c r="D110" s="2"/>
@@ -14237,8 +14380,10 @@
       <c r="BJ110" s="3"/>
       <c r="BK110" s="3"/>
     </row>
-    <row r="111" spans="1:63" ht="15" customHeight="1">
-      <c r="A111" s="3"/>
+    <row r="111" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A111" s="10">
+        <v>424</v>
+      </c>
       <c r="B111" s="2"/>
       <c r="C111" s="2"/>
       <c r="D111" s="2"/>
@@ -14351,8 +14496,10 @@
       <c r="BJ111" s="3"/>
       <c r="BK111" s="3"/>
     </row>
-    <row r="112" spans="1:63" ht="15" customHeight="1">
-      <c r="A112" s="3"/>
+    <row r="112" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A112" s="10">
+        <v>425</v>
+      </c>
       <c r="B112" s="2"/>
       <c r="C112" s="2"/>
       <c r="D112" s="2"/>
@@ -14416,8 +14563,10 @@
       <c r="BJ112" s="3"/>
       <c r="BK112" s="3"/>
     </row>
-    <row r="113" spans="1:63" ht="15" customHeight="1">
-      <c r="A113" s="3"/>
+    <row r="113" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A113" s="10">
+        <v>429</v>
+      </c>
       <c r="B113" s="2"/>
       <c r="C113" s="2"/>
       <c r="D113" s="2"/>
@@ -14508,8 +14657,10 @@
       <c r="BJ113" s="3"/>
       <c r="BK113" s="3"/>
     </row>
-    <row r="114" spans="1:63" ht="15" customHeight="1">
-      <c r="A114" s="3"/>
+    <row r="114" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A114" s="10">
+        <v>437</v>
+      </c>
       <c r="B114" s="2"/>
       <c r="C114" s="2"/>
       <c r="D114" s="2"/>
@@ -14619,8 +14770,10 @@
       <c r="BJ114" s="3"/>
       <c r="BK114" s="3"/>
     </row>
-    <row r="115" spans="1:63" ht="15" customHeight="1">
-      <c r="A115" s="3"/>
+    <row r="115" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A115" s="10">
+        <v>438</v>
+      </c>
       <c r="B115" s="2"/>
       <c r="C115" s="2"/>
       <c r="D115" s="2"/>
@@ -14684,8 +14837,10 @@
       <c r="BJ115" s="3"/>
       <c r="BK115" s="3"/>
     </row>
-    <row r="116" spans="1:63" ht="15" customHeight="1">
-      <c r="A116" s="3"/>
+    <row r="116" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A116" s="10">
+        <v>439</v>
+      </c>
       <c r="B116" s="2"/>
       <c r="C116" s="2"/>
       <c r="D116" s="2"/>
@@ -14787,8 +14942,10 @@
       <c r="BJ116" s="3"/>
       <c r="BK116" s="3"/>
     </row>
-    <row r="117" spans="1:63" ht="15" customHeight="1">
-      <c r="A117" s="3"/>
+    <row r="117" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A117" s="10">
+        <v>440</v>
+      </c>
       <c r="B117" s="2"/>
       <c r="C117" s="2"/>
       <c r="D117" s="2"/>
@@ -14852,8 +15009,10 @@
       <c r="BJ117" s="3"/>
       <c r="BK117" s="3"/>
     </row>
-    <row r="118" spans="1:63" ht="15" customHeight="1">
-      <c r="A118" s="3"/>
+    <row r="118" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A118" s="10">
+        <v>448</v>
+      </c>
       <c r="B118" s="2"/>
       <c r="C118" s="2"/>
       <c r="D118" s="2"/>
@@ -14963,8 +15122,10 @@
       <c r="BJ118" s="3"/>
       <c r="BK118" s="3"/>
     </row>
-    <row r="119" spans="1:63" ht="15" customHeight="1">
-      <c r="A119" s="3"/>
+    <row r="119" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A119" s="10">
+        <v>449</v>
+      </c>
       <c r="B119" s="2"/>
       <c r="C119" s="2"/>
       <c r="D119" s="2"/>
@@ -15077,8 +15238,10 @@
       <c r="BJ119" s="3"/>
       <c r="BK119" s="3"/>
     </row>
-    <row r="120" spans="1:63" ht="15" customHeight="1">
-      <c r="A120" s="3"/>
+    <row r="120" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A120" s="10">
+        <v>450</v>
+      </c>
       <c r="B120" s="2"/>
       <c r="C120" s="2"/>
       <c r="D120" s="2"/>
@@ -15191,8 +15354,10 @@
       <c r="BJ120" s="3"/>
       <c r="BK120" s="3"/>
     </row>
-    <row r="121" spans="1:63" ht="15" customHeight="1">
-      <c r="A121" s="3"/>
+    <row r="121" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A121" s="10">
+        <v>451</v>
+      </c>
       <c r="B121" s="2"/>
       <c r="C121" s="2"/>
       <c r="D121" s="2"/>
@@ -15305,8 +15470,10 @@
       <c r="BJ121" s="3"/>
       <c r="BK121" s="3"/>
     </row>
-    <row r="122" spans="1:63" ht="15" customHeight="1">
-      <c r="A122" s="3"/>
+    <row r="122" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A122" s="10">
+        <v>452</v>
+      </c>
       <c r="B122" s="2"/>
       <c r="C122" s="2"/>
       <c r="D122" s="2"/>
@@ -15419,8 +15586,10 @@
       <c r="BJ122" s="3"/>
       <c r="BK122" s="3"/>
     </row>
-    <row r="123" spans="1:63" ht="15" customHeight="1">
-      <c r="A123" s="3"/>
+    <row r="123" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A123" s="10">
+        <v>454</v>
+      </c>
       <c r="B123" s="2"/>
       <c r="C123" s="2"/>
       <c r="D123" s="2"/>
@@ -15533,8 +15702,10 @@
       <c r="BJ123" s="3"/>
       <c r="BK123" s="3"/>
     </row>
-    <row r="124" spans="1:63" ht="15" customHeight="1">
-      <c r="A124" s="3"/>
+    <row r="124" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A124" s="10">
+        <v>456</v>
+      </c>
       <c r="B124" s="2"/>
       <c r="C124" s="2"/>
       <c r="D124" s="2"/>
@@ -15641,8 +15812,10 @@
       <c r="BJ124" s="3"/>
       <c r="BK124" s="3"/>
     </row>
-    <row r="125" spans="1:63" ht="15" customHeight="1">
-      <c r="A125" s="3"/>
+    <row r="125" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A125" s="10">
+        <v>457</v>
+      </c>
       <c r="B125" s="2"/>
       <c r="C125" s="2"/>
       <c r="D125" s="2"/>
@@ -15755,8 +15928,10 @@
       <c r="BJ125" s="3"/>
       <c r="BK125" s="3"/>
     </row>
-    <row r="126" spans="1:63" ht="15" customHeight="1">
-      <c r="A126" s="3"/>
+    <row r="126" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A126" s="10">
+        <v>458</v>
+      </c>
       <c r="B126" s="2"/>
       <c r="C126" s="2"/>
       <c r="D126" s="2"/>
@@ -15869,8 +16044,10 @@
       <c r="BJ126" s="3"/>
       <c r="BK126" s="3"/>
     </row>
-    <row r="127" spans="1:63" ht="15" customHeight="1">
-      <c r="A127" s="3"/>
+    <row r="127" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A127" s="10">
+        <v>459</v>
+      </c>
       <c r="B127" s="2"/>
       <c r="C127" s="2"/>
       <c r="D127" s="2"/>
@@ -15980,8 +16157,10 @@
       <c r="BJ127" s="3"/>
       <c r="BK127" s="3"/>
     </row>
-    <row r="128" spans="1:63" ht="15" customHeight="1">
-      <c r="A128" s="3"/>
+    <row r="128" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A128" s="10">
+        <v>460</v>
+      </c>
       <c r="B128" s="2"/>
       <c r="C128" s="2"/>
       <c r="D128" s="2"/>
@@ -16088,8 +16267,10 @@
       <c r="BJ128" s="3"/>
       <c r="BK128" s="3"/>
     </row>
-    <row r="129" spans="1:63" ht="15" customHeight="1">
-      <c r="A129" s="3"/>
+    <row r="129" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A129" s="10">
+        <v>462</v>
+      </c>
       <c r="B129" s="2"/>
       <c r="C129" s="2"/>
       <c r="D129" s="2"/>
@@ -16205,8 +16386,10 @@
       <c r="BJ129" s="3"/>
       <c r="BK129" s="3"/>
     </row>
-    <row r="130" spans="1:63" ht="15" customHeight="1">
-      <c r="A130" s="3"/>
+    <row r="130" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A130" s="10">
+        <v>463</v>
+      </c>
       <c r="B130" s="2"/>
       <c r="C130" s="2"/>
       <c r="D130" s="2"/>
@@ -16316,8 +16499,10 @@
       <c r="BJ130" s="3"/>
       <c r="BK130" s="3"/>
     </row>
-    <row r="131" spans="1:63" ht="15" customHeight="1">
-      <c r="A131" s="3"/>
+    <row r="131" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A131" s="10">
+        <v>465</v>
+      </c>
       <c r="B131" s="2"/>
       <c r="C131" s="2"/>
       <c r="D131" s="2"/>
@@ -16427,8 +16612,10 @@
       <c r="BJ131" s="3"/>
       <c r="BK131" s="3"/>
     </row>
-    <row r="132" spans="1:63" ht="15" customHeight="1">
-      <c r="A132" s="3"/>
+    <row r="132" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A132" s="10">
+        <v>467</v>
+      </c>
       <c r="B132" s="2"/>
       <c r="C132" s="2"/>
       <c r="D132" s="2"/>
@@ -16509,7 +16696,7 @@
       <c r="AO132" s="3" t="s">
         <v>592</v>
       </c>
-      <c r="AP132" s="10">
+      <c r="AP132" s="3">
         <v>0.5</v>
       </c>
       <c r="AQ132" s="3">
@@ -16538,8 +16725,10 @@
       <c r="BJ132" s="3"/>
       <c r="BK132" s="3"/>
     </row>
-    <row r="133" spans="1:63" ht="15" customHeight="1">
-      <c r="A133" s="3"/>
+    <row r="133" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A133" s="10">
+        <v>468</v>
+      </c>
       <c r="B133" s="2"/>
       <c r="C133" s="2"/>
       <c r="D133" s="2"/>
@@ -16578,7 +16767,7 @@
         <v>0.5</v>
       </c>
       <c r="T133" s="4">
-        <f t="shared" ref="T132:T144" si="10">SUM(Q133:S133)</f>
+        <f t="shared" ref="T133:T144" si="10">SUM(Q133:S133)</f>
         <v>2.5</v>
       </c>
       <c r="U133" s="3" t="s">
@@ -16652,8 +16841,10 @@
       <c r="BJ133" s="3"/>
       <c r="BK133" s="3"/>
     </row>
-    <row r="134" spans="1:63" ht="15" customHeight="1">
-      <c r="A134" s="3"/>
+    <row r="134" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A134" s="10">
+        <v>470</v>
+      </c>
       <c r="B134" s="2"/>
       <c r="C134" s="2"/>
       <c r="D134" s="2"/>
@@ -16734,7 +16925,7 @@
       <c r="AO134" s="3" t="s">
         <v>602</v>
       </c>
-      <c r="AP134" s="10">
+      <c r="AP134" s="3">
         <v>0.5</v>
       </c>
       <c r="AQ134" s="3">
@@ -16763,8 +16954,10 @@
       <c r="BJ134" s="3"/>
       <c r="BK134" s="3"/>
     </row>
-    <row r="135" spans="1:63" ht="15" customHeight="1">
-      <c r="A135" s="3"/>
+    <row r="135" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A135" s="10">
+        <v>471</v>
+      </c>
       <c r="B135" s="2"/>
       <c r="C135" s="2"/>
       <c r="D135" s="2"/>
@@ -16874,8 +17067,10 @@
       <c r="BJ135" s="3"/>
       <c r="BK135" s="3"/>
     </row>
-    <row r="136" spans="1:63" ht="15" customHeight="1">
-      <c r="A136" s="3"/>
+    <row r="136" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A136" s="10">
+        <v>472</v>
+      </c>
       <c r="B136" s="2"/>
       <c r="C136" s="2"/>
       <c r="D136" s="2"/>
@@ -16988,8 +17183,10 @@
       <c r="BJ136" s="3"/>
       <c r="BK136" s="3"/>
     </row>
-    <row r="137" spans="1:63" ht="15" customHeight="1">
-      <c r="A137" s="3"/>
+    <row r="137" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A137" s="10">
+        <v>473</v>
+      </c>
       <c r="B137" s="2"/>
       <c r="C137" s="2"/>
       <c r="D137" s="2"/>
@@ -17099,8 +17296,10 @@
       <c r="BJ137" s="3"/>
       <c r="BK137" s="3"/>
     </row>
-    <row r="138" spans="1:63" ht="15" customHeight="1">
-      <c r="A138" s="3"/>
+    <row r="138" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A138" s="10">
+        <v>474</v>
+      </c>
       <c r="B138" s="2"/>
       <c r="C138" s="2"/>
       <c r="D138" s="2"/>
@@ -17210,8 +17409,10 @@
       <c r="BJ138" s="3"/>
       <c r="BK138" s="3"/>
     </row>
-    <row r="139" spans="1:63" ht="15" customHeight="1">
-      <c r="A139" s="3"/>
+    <row r="139" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A139" s="10">
+        <v>475</v>
+      </c>
       <c r="B139" s="2"/>
       <c r="C139" s="2"/>
       <c r="D139" s="2"/>
@@ -17321,8 +17522,10 @@
       <c r="BJ139" s="3"/>
       <c r="BK139" s="3"/>
     </row>
-    <row r="140" spans="1:63" ht="15" customHeight="1">
-      <c r="A140" s="3"/>
+    <row r="140" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A140" s="10">
+        <v>476</v>
+      </c>
       <c r="B140" s="2"/>
       <c r="C140" s="2"/>
       <c r="D140" s="2"/>
@@ -17435,8 +17638,10 @@
       <c r="BJ140" s="3"/>
       <c r="BK140" s="3"/>
     </row>
-    <row r="141" spans="1:63" ht="15" customHeight="1">
-      <c r="A141" s="3"/>
+    <row r="141" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A141" s="10">
+        <v>477</v>
+      </c>
       <c r="B141" s="2"/>
       <c r="C141" s="2"/>
       <c r="D141" s="2"/>
@@ -17549,8 +17754,10 @@
       <c r="BJ141" s="3"/>
       <c r="BK141" s="3"/>
     </row>
-    <row r="142" spans="1:63" ht="15" customHeight="1">
-      <c r="A142" s="3"/>
+    <row r="142" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A142" s="10">
+        <v>478</v>
+      </c>
       <c r="B142" s="2"/>
       <c r="C142" s="2"/>
       <c r="D142" s="2"/>
@@ -17660,8 +17867,10 @@
       <c r="BJ142" s="3"/>
       <c r="BK142" s="3"/>
     </row>
-    <row r="143" spans="1:63" ht="15" customHeight="1">
-      <c r="A143" s="3"/>
+    <row r="143" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A143" s="10">
+        <v>479</v>
+      </c>
       <c r="B143" s="2"/>
       <c r="C143" s="2"/>
       <c r="D143" s="2"/>
@@ -17774,8 +17983,10 @@
       <c r="BJ143" s="3"/>
       <c r="BK143" s="3"/>
     </row>
-    <row r="144" spans="1:63" ht="15" customHeight="1">
-      <c r="A144" s="3"/>
+    <row r="144" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A144" s="10">
+        <v>480</v>
+      </c>
       <c r="B144" s="2"/>
       <c r="C144" s="2"/>
       <c r="D144" s="2"/>
@@ -17888,8 +18099,10 @@
       <c r="BJ144" s="3"/>
       <c r="BK144" s="3"/>
     </row>
-    <row r="145" spans="1:63" ht="15" customHeight="1">
-      <c r="A145" s="3"/>
+    <row r="145" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A145" s="10">
+        <v>481</v>
+      </c>
       <c r="B145" s="2"/>
       <c r="C145" s="2"/>
       <c r="D145" s="2"/>
@@ -17999,8 +18212,10 @@
       <c r="BJ145" s="3"/>
       <c r="BK145" s="3"/>
     </row>
-    <row r="146" spans="1:63" ht="15" customHeight="1">
-      <c r="A146" s="3"/>
+    <row r="146" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A146" s="10">
+        <v>491</v>
+      </c>
       <c r="B146" s="2"/>
       <c r="C146" s="2"/>
       <c r="D146" s="2"/>
@@ -18064,8 +18279,10 @@
       <c r="BJ146" s="3"/>
       <c r="BK146" s="3"/>
     </row>
-    <row r="147" spans="1:63" ht="15" customHeight="1">
-      <c r="A147" s="3"/>
+    <row r="147" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A147" s="10">
+        <v>492</v>
+      </c>
       <c r="B147" s="2"/>
       <c r="C147" s="2"/>
       <c r="D147" s="2"/>
@@ -18170,7 +18387,7 @@
       <c r="BJ147" s="3"/>
       <c r="BK147" s="3"/>
     </row>
-    <row r="148" spans="1:63" ht="15" customHeight="1">
+    <row r="148" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A148" s="3"/>
       <c r="B148" s="2"/>
       <c r="C148" s="2"/>
@@ -18235,7 +18452,7 @@
       <c r="BJ148" s="3"/>
       <c r="BK148" s="3"/>
     </row>
-    <row r="149" spans="1:63" ht="15" customHeight="1">
+    <row r="149" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A149" s="3"/>
       <c r="B149" s="2"/>
       <c r="C149" s="2"/>
@@ -18300,7 +18517,7 @@
       <c r="BJ149" s="3"/>
       <c r="BK149" s="3"/>
     </row>
-    <row r="150" spans="1:63" ht="15" customHeight="1">
+    <row r="150" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A150" s="5"/>
       <c r="B150" s="7"/>
       <c r="C150" s="7"/>
@@ -18365,7 +18582,7 @@
       <c r="BJ150" s="5"/>
       <c r="BK150" s="3"/>
     </row>
-    <row r="151" spans="1:63" ht="15" customHeight="1">
+    <row r="151" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A151" s="5"/>
       <c r="B151" s="7"/>
       <c r="C151" s="7"/>
@@ -18430,7 +18647,7 @@
       <c r="BJ151" s="5"/>
       <c r="BK151" s="3"/>
     </row>
-    <row r="152" spans="1:63" ht="15" customHeight="1">
+    <row r="152" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A152" s="5"/>
       <c r="B152" s="7"/>
       <c r="C152" s="7"/>
@@ -18495,7 +18712,7 @@
       <c r="BJ152" s="5"/>
       <c r="BK152" s="3"/>
     </row>
-    <row r="153" spans="1:63" ht="15" customHeight="1">
+    <row r="153" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A153" s="5"/>
       <c r="B153" s="7"/>
       <c r="C153" s="7"/>
@@ -18560,7 +18777,7 @@
       <c r="BJ153" s="5"/>
       <c r="BK153" s="3"/>
     </row>
-    <row r="154" spans="1:63" ht="15" customHeight="1">
+    <row r="154" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A154" s="3"/>
       <c r="B154" s="2"/>
       <c r="C154" s="2"/>
@@ -18625,7 +18842,7 @@
       <c r="BJ154" s="3"/>
       <c r="BK154" s="3"/>
     </row>
-    <row r="155" spans="1:63" ht="15" customHeight="1">
+    <row r="155" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A155" s="3"/>
       <c r="B155" s="2"/>
       <c r="C155" s="2"/>
@@ -18690,7 +18907,7 @@
       <c r="BJ155" s="3"/>
       <c r="BK155" s="3"/>
     </row>
-    <row r="156" spans="1:63" ht="15" customHeight="1">
+    <row r="156" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A156" s="3"/>
       <c r="B156" s="2"/>
       <c r="C156" s="2"/>
@@ -18755,7 +18972,7 @@
       <c r="BJ156" s="3"/>
       <c r="BK156" s="3"/>
     </row>
-    <row r="157" spans="1:63" ht="15" customHeight="1">
+    <row r="157" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A157" s="3"/>
       <c r="B157" s="2"/>
       <c r="C157" s="2"/>
@@ -18820,7 +19037,7 @@
       <c r="BJ157" s="3"/>
       <c r="BK157" s="3"/>
     </row>
-    <row r="158" spans="1:63" ht="15" customHeight="1">
+    <row r="158" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A158" s="3"/>
       <c r="B158" s="2"/>
       <c r="C158" s="2"/>
@@ -18885,7 +19102,7 @@
       <c r="BJ158" s="3"/>
       <c r="BK158" s="3"/>
     </row>
-    <row r="159" spans="1:63" ht="15" customHeight="1">
+    <row r="159" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A159" s="3"/>
       <c r="B159" s="2"/>
       <c r="C159" s="2"/>
@@ -18950,7 +19167,7 @@
       <c r="BJ159" s="3"/>
       <c r="BK159" s="3"/>
     </row>
-    <row r="160" spans="1:63" ht="15" customHeight="1">
+    <row r="160" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A160" s="3"/>
       <c r="B160" s="2"/>
       <c r="C160" s="2"/>
@@ -19015,7 +19232,7 @@
       <c r="BJ160" s="3"/>
       <c r="BK160" s="3"/>
     </row>
-    <row r="161" spans="1:63" ht="15" customHeight="1">
+    <row r="161" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A161" s="3"/>
       <c r="B161" s="2"/>
       <c r="C161" s="2"/>
@@ -19080,7 +19297,7 @@
       <c r="BJ161" s="3"/>
       <c r="BK161" s="3"/>
     </row>
-    <row r="162" spans="1:63" ht="15" customHeight="1">
+    <row r="162" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A162" s="3"/>
       <c r="B162" s="2"/>
       <c r="C162" s="2"/>
@@ -19145,7 +19362,7 @@
       <c r="BJ162" s="3"/>
       <c r="BK162" s="3"/>
     </row>
-    <row r="163" spans="1:63" ht="15" customHeight="1">
+    <row r="163" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A163" s="3"/>
       <c r="B163" s="2"/>
       <c r="C163" s="2"/>
@@ -19210,7 +19427,7 @@
       <c r="BJ163" s="3"/>
       <c r="BK163" s="3"/>
     </row>
-    <row r="164" spans="1:63" ht="15" customHeight="1">
+    <row r="164" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A164" s="3"/>
       <c r="B164" s="2"/>
       <c r="C164" s="2"/>

</xml_diff>